<commit_message>
Removed class declarations overriding Typed descriptors
</commit_message>
<xml_diff>
--- a/docs/examples/customization.xlsx
+++ b/docs/examples/customization.xlsx
@@ -60,16 +60,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font/>
     <font>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
     </font>
     <font>
+      <sz val="20"/>
+    </font>
+    <font/>
+    <font>
       <color rgb="FF777777"/>
-    </font>
-    <font>
-      <sz val="20"/>
     </font>
   </fonts>
   <fills count="3">
@@ -96,36 +96,36 @@
   </borders>
   <cellStyleXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="2"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="2"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="6">
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="3">
       <protection hidden="0" locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="Row, text" xfId="1"/>
-    <cellStyle hidden="0" name="Row" xfId="2"/>
-    <cellStyle hidden="0" name="Header" xfId="3"/>
+    <cellStyle hidden="0" name="Header" xfId="1"/>
+    <cellStyle hidden="0" name="Title" xfId="2"/>
+    <cellStyle hidden="0" name="Row, decimal" xfId="3"/>
     <cellStyle hidden="0" name="Description" xfId="4"/>
-    <cellStyle hidden="0" name="Title" xfId="5"/>
-    <cellStyle hidden="0" name="Row, decimal" xfId="6"/>
+    <cellStyle hidden="0" name="Row, text" xfId="5"/>
+    <cellStyle hidden="0" name="Row" xfId="6"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>

</xml_diff>

<commit_message>
Column testing and multiple bugfixes
</commit_message>
<xml_diff>
--- a/docs/examples/customization.xlsx
+++ b/docs/examples/customization.xlsx
@@ -61,15 +61,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="20"/>
     </font>
     <font>
-      <sz val="20"/>
+      <color rgb="FF777777"/>
     </font>
     <font/>
     <font>
-      <color rgb="FF777777"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
     </font>
   </fonts>
   <fills count="3">
@@ -96,21 +96,21 @@
   </borders>
   <cellStyleXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="2"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6"/>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="5">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="0"/>
     </xf>
@@ -120,12 +120,12 @@
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="Header" xfId="1"/>
-    <cellStyle hidden="0" name="Title" xfId="2"/>
+    <cellStyle hidden="0" name="Title" xfId="1"/>
+    <cellStyle hidden="0" name="Description" xfId="2"/>
     <cellStyle hidden="0" name="Row, decimal" xfId="3"/>
-    <cellStyle hidden="0" name="Description" xfId="4"/>
-    <cellStyle hidden="0" name="Row, text" xfId="5"/>
-    <cellStyle hidden="0" name="Row" xfId="6"/>
+    <cellStyle hidden="0" name="Row, text" xfId="4"/>
+    <cellStyle hidden="0" name="Row" xfId="5"/>
+    <cellStyle hidden="0" name="Header" xfId="6"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>

</xml_diff>

<commit_message>
Restored python 3 compatibility
</commit_message>
<xml_diff>
--- a/docs/examples/customization.xlsx
+++ b/docs/examples/customization.xlsx
@@ -62,14 +62,14 @@
     </font>
     <font/>
     <font>
-      <sz val="20"/>
-    </font>
-    <font>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
     </font>
     <font>
       <color rgb="FF777777"/>
+    </font>
+    <font>
+      <sz val="20"/>
     </font>
   </fonts>
   <fills count="3">
@@ -82,6 +82,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF1a1f43"/>
+        <bgColor rgb="FF1a1f43"/>
       </patternFill>
     </fill>
   </fills>
@@ -96,36 +97,31 @@
   </borders>
   <cellStyleXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="2"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="2"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
-      <protection hidden="0" locked="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="6">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="5">
-      <protection hidden="0" locked="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="Row, text" xfId="1"/>
-    <cellStyle hidden="0" name="Title" xfId="2"/>
-    <cellStyle hidden="0" name="Header" xfId="3"/>
+    <cellStyle hidden="0" name="Row" xfId="1"/>
+    <cellStyle hidden="0" name="Header" xfId="2"/>
+    <cellStyle hidden="0" name="Row, decimal" xfId="3"/>
     <cellStyle hidden="0" name="Description" xfId="4"/>
-    <cellStyle hidden="0" name="Row, decimal" xfId="5"/>
-    <cellStyle hidden="0" name="Row" xfId="6"/>
+    <cellStyle hidden="0" name="Title" xfId="5"/>
+    <cellStyle hidden="0" name="Row, text" xfId="6"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>

</xml_diff>